<commit_message>
scss 적용, redux 조사
</commit_message>
<xml_diff>
--- a/document/환경구축.xlsx
+++ b/document/환경구축.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepo\react_calendar\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571512EE-A6B5-4B99-B224-8FA235EF58DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126A0D67-346D-47B0-B4DA-C8E3385E79C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13965" yWindow="4605" windowWidth="23265" windowHeight="9300" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18885" yWindow="3150" windowWidth="23265" windowHeight="9300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="목표" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>REACT PROJECT 생성</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -174,10 +174,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">:기존 Date함수는 </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>참조URL:https://momentjs.com/</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -221,6 +217,25 @@
   </si>
   <si>
     <t>npm, yarn을 전역설정해주었다. 패키지 내에서만 설정해서 3일간 잘 되었으나 어느순간 되지 않았다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>redux 스토어 관련</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://deminoth.github.io/redux/basics/Reducers.html</t>
+  </si>
+  <si>
+    <t>2.Redux</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>:기존 Date함수는 원하는 결과까지 처리가 너무 많다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>:가장 사용률이 높은 상태관리 라이브러리.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -328,7 +343,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -339,6 +354,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -731,17 +747,17 @@
     </row>
     <row r="13" spans="2:3">
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:3">
       <c r="C14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:3">
       <c r="C15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -753,10 +769,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8DB5DE8-7419-4EDA-B549-8F1AF8520178}">
-  <dimension ref="B1:C7"/>
+  <dimension ref="B1:C11"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -777,17 +793,28 @@
     </row>
     <row r="4" spans="2:3">
       <c r="C4" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="C11" s="8" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -826,7 +853,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -876,7 +903,7 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -901,12 +928,12 @@
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="2:2">
       <c r="B3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -921,25 +948,37 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A92952F4-FDDA-4D76-9437-43503456CBC6}">
-  <dimension ref="A2"/>
+  <dimension ref="A2:A5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{BC512D7F-612A-4E17-BF66-292392FEE4BD}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{70990C68-8A53-4336-8242-782C26C4192C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -947,7 +986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0280C57F-C9A6-4D93-83C0-D022EF0A9790}">
   <dimension ref="B2:C4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -959,17 +998,17 @@
   <sheetData>
     <row r="2" spans="2:3">
       <c r="B2" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="2:3">
       <c r="C3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="2:3">
       <c r="C4" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>